<commit_message>
prepare for public release
</commit_message>
<xml_diff>
--- a/source/data/debrief_responses.xlsx
+++ b/source/data/debrief_responses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayhuang/Documents/Blueprint_Labs/radiology_ai_data-git/source/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{76FCB339-D00A-8E42-A155-F5B415383DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99246B63-DAF1-D24E-B91F-65FFADA83AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="2300" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,16 +16,11 @@
     <sheet name="debrief_responses" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="7362" uniqueCount="1548">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7362" uniqueCount="1548">
   <si>
     <t>vietnam_pilot1</t>
   </si>
@@ -4919,7 +4914,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -5239,15 +5234,15 @@
   </fills>
   <borders count="10">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -5255,8 +5250,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
@@ -5264,8 +5259,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.39997558519241921"/>
@@ -5273,12 +5268,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF7F7F7F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -5288,12 +5283,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -5303,8 +5298,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -5312,12 +5307,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="double">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="double">
+      </left>
+      <right style="double">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -5327,12 +5322,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FFB2B2B2"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
@@ -5342,8 +5337,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -5461,7 +5456,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -5614,25 +5609,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110%"/>
-                <a:satMod val="105%"/>
-                <a:tint val="67%"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="103%"/>
-                <a:tint val="73%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="109%"/>
-                <a:tint val="81%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -5640,25 +5635,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103%"/>
-                <a:lumMod val="102%"/>
-                <a:tint val="94%"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110%"/>
-                <a:lumMod val="100%"/>
-                <a:shade val="100%"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99%"/>
-                <a:satMod val="120%"/>
-                <a:shade val="78%"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -5671,21 +5666,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -5699,7 +5694,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63%"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -5711,32 +5706,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95%"/>
-            <a:satMod val="170%"/>
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93%"/>
-                <a:satMod val="150%"/>
-                <a:shade val="98%"/>
-                <a:lumMod val="102%"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="98%"/>
-                <a:satMod val="130%"/>
-                <a:shade val="90%"/>
-                <a:lumMod val="103%"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63%"/>
-                <a:satMod val="120%"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -5756,7 +5751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:KK36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
@@ -16550,7 +16545,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="19" spans="1:297" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:297" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1240</v>
       </c>

</xml_diff>